<commit_message>
[308] Làm gọn code xuất Excel
</commit_message>
<xml_diff>
--- a/KnowledgeSystem/AppResources/308_Statistic.xlsx
+++ b/KnowledgeSystem/AppResources/308_Statistic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01. Softwares Programming\24. Knowledge System\01. Projects\KnowledgeSystem\KnowledgeSystem\AppResources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DBA022-2722-438A-9933-A4C3995C1D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613014CA-9787-496F-AD59-84A5A358D45D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="4470" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phụ lục 2" sheetId="1" r:id="rId1"/>
@@ -23,23 +23,34 @@
     <sheet name="Biểu mẫu 7" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'Biểu mẫu 3'!$A$1:$AD$6</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Biểu mẫu 3'!$A$1:$AD$25</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'Biểu mẫu 4'!$A$1:$Z$1</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">'Biểu mẫu 5'!$A$1:$Z$1</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="6">'Biểu mẫu 6'!$A$1:$Z$1</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="7">'Biểu mẫu 7'!$A$1:$Z$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="74">
   <si>
     <t>Tên cơ sở lao động: Phòng thử nghiệm Vật lý - Bộ phận Kĩ thuật luyện kim - Công ty TNHH Gang Thép Hưng Nghiệp Formosa Hà Tĩnh</t>
   </si>
@@ -780,6 +791,60 @@
   </si>
   <si>
     <t>III. Các trường hợp tai nạn lao động</t>
+  </si>
+  <si>
+    <t>Tai nạn lao động</t>
+  </si>
+  <si>
+    <t>Cộng</t>
+  </si>
+  <si>
+    <t>表單三: 報告時間中勞工疾病情形</t>
+  </si>
+  <si>
+    <t>項次</t>
+  </si>
+  <si>
+    <t>疾病類型</t>
+  </si>
+  <si>
+    <t>第一季</t>
+  </si>
+  <si>
+    <t>第二季</t>
+  </si>
+  <si>
+    <t>第三季</t>
+  </si>
+  <si>
+    <t>第四季</t>
+  </si>
+  <si>
+    <t>I. 得一般疾病之人數:</t>
+  </si>
+  <si>
+    <t>II. 得職業病之人數</t>
+  </si>
+  <si>
+    <t>III. 勞動職災件數</t>
+  </si>
+  <si>
+    <t>勞動職災</t>
+  </si>
+  <si>
+    <t>總計</t>
+  </si>
+  <si>
+    <t>件數</t>
+  </si>
+  <si>
+    <t>死亡</t>
+  </si>
+  <si>
+    <t>Bệnh nghề nghiệp</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -904,7 +969,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -927,57 +992,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1011,14 +1030,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1029,41 +1045,35 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1391,34 +1401,34 @@
       <c r="Z1" s="14"/>
     </row>
     <row r="2" spans="1:31" ht="20.100000000000001" customHeight="1">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16"/>
-      <c r="X2" s="16"/>
-      <c r="Y2" s="16"/>
-      <c r="Z2" s="16"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
     </row>
     <row r="3" spans="1:31" ht="18.75">
       <c r="A3" s="6"/>
@@ -1449,34 +1459,34 @@
       <c r="Z3" s="6"/>
     </row>
     <row r="4" spans="1:31" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="18"/>
-      <c r="T4" s="18"/>
-      <c r="U4" s="18"/>
-      <c r="V4" s="18"/>
-      <c r="W4" s="18"/>
-      <c r="X4" s="18"/>
-      <c r="Y4" s="18"/>
-      <c r="Z4" s="18"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17"/>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
@@ -1484,34 +1494,34 @@
       <c r="AE4" s="2"/>
     </row>
     <row r="5" spans="1:31" s="1" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="18"/>
-      <c r="S5" s="18"/>
-      <c r="T5" s="18"/>
-      <c r="U5" s="18"/>
-      <c r="V5" s="18"/>
-      <c r="W5" s="18"/>
-      <c r="X5" s="18"/>
-      <c r="Y5" s="18"/>
-      <c r="Z5" s="18"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="17"/>
+      <c r="W5" s="17"/>
+      <c r="X5" s="17"/>
+      <c r="Y5" s="17"/>
+      <c r="Z5" s="17"/>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
@@ -1519,34 +1529,34 @@
       <c r="AE5" s="2"/>
     </row>
     <row r="6" spans="1:31" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="18"/>
-      <c r="T6" s="18"/>
-      <c r="U6" s="18"/>
-      <c r="V6" s="18"/>
-      <c r="W6" s="18"/>
-      <c r="X6" s="18"/>
-      <c r="Y6" s="18"/>
-      <c r="Z6" s="18"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="17"/>
+      <c r="U6" s="17"/>
+      <c r="V6" s="17"/>
+      <c r="W6" s="17"/>
+      <c r="X6" s="17"/>
+      <c r="Y6" s="17"/>
+      <c r="Z6" s="17"/>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
@@ -1554,36 +1564,36 @@
       <c r="AE6" s="2"/>
     </row>
     <row r="7" spans="1:31" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="18"/>
-      <c r="U7" s="18"/>
-      <c r="V7" s="18"/>
-      <c r="W7" s="18"/>
-      <c r="X7" s="18"/>
-      <c r="Y7" s="18"/>
-      <c r="Z7" s="18"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="17"/>
+      <c r="U7" s="17"/>
+      <c r="V7" s="17"/>
+      <c r="W7" s="17"/>
+      <c r="X7" s="17"/>
+      <c r="Y7" s="17"/>
+      <c r="Z7" s="17"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
@@ -1591,36 +1601,36 @@
       <c r="AE7" s="2"/>
     </row>
     <row r="8" spans="1:31" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18" t="s">
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="18"/>
-      <c r="T8" s="18"/>
-      <c r="U8" s="18"/>
-      <c r="V8" s="18"/>
-      <c r="W8" s="18"/>
-      <c r="X8" s="18"/>
-      <c r="Y8" s="18"/>
-      <c r="Z8" s="18"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="17"/>
+      <c r="U8" s="17"/>
+      <c r="V8" s="17"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="17"/>
+      <c r="Y8" s="17"/>
+      <c r="Z8" s="17"/>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
@@ -1628,34 +1638,34 @@
       <c r="AE8" s="2"/>
     </row>
     <row r="9" spans="1:31" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
-      <c r="S9" s="18"/>
-      <c r="T9" s="18"/>
-      <c r="U9" s="18"/>
-      <c r="V9" s="18"/>
-      <c r="W9" s="18"/>
-      <c r="X9" s="18"/>
-      <c r="Y9" s="18"/>
-      <c r="Z9" s="18"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="17"/>
+      <c r="U9" s="17"/>
+      <c r="V9" s="17"/>
+      <c r="W9" s="17"/>
+      <c r="X9" s="17"/>
+      <c r="Y9" s="17"/>
+      <c r="Z9" s="17"/>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
@@ -1663,34 +1673,34 @@
       <c r="AE9" s="2"/>
     </row>
     <row r="10" spans="1:31" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
-      <c r="T10" s="18"/>
-      <c r="U10" s="18"/>
-      <c r="V10" s="18"/>
-      <c r="W10" s="18"/>
-      <c r="X10" s="18"/>
-      <c r="Y10" s="18"/>
-      <c r="Z10" s="18"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="17"/>
+      <c r="U10" s="17"/>
+      <c r="V10" s="17"/>
+      <c r="W10" s="17"/>
+      <c r="X10" s="17"/>
+      <c r="Y10" s="17"/>
+      <c r="Z10" s="17"/>
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
@@ -1796,38 +1806,38 @@
       <c r="AE13" s="2"/>
     </row>
     <row r="14" spans="1:31" s="4" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17" t="s">
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="17" t="s">
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="T14" s="17"/>
-      <c r="U14" s="17"/>
-      <c r="V14" s="17"/>
-      <c r="W14" s="17"/>
-      <c r="X14" s="17"/>
-      <c r="Y14" s="17"/>
-      <c r="Z14" s="17"/>
+      <c r="T14" s="16"/>
+      <c r="U14" s="16"/>
+      <c r="V14" s="16"/>
+      <c r="W14" s="16"/>
+      <c r="X14" s="16"/>
+      <c r="Y14" s="16"/>
+      <c r="Z14" s="16"/>
       <c r="AA14" s="3"/>
       <c r="AB14" s="3"/>
       <c r="AC14" s="3"/>
@@ -1865,34 +1875,34 @@
       <c r="Z15" s="14"/>
     </row>
     <row r="16" spans="1:31" ht="24.95" customHeight="1">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
-      <c r="U16" s="15"/>
-      <c r="V16" s="15"/>
-      <c r="W16" s="15"/>
-      <c r="X16" s="15"/>
-      <c r="Y16" s="15"/>
-      <c r="Z16" s="15"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
+      <c r="T16" s="19"/>
+      <c r="U16" s="19"/>
+      <c r="V16" s="19"/>
+      <c r="W16" s="19"/>
+      <c r="X16" s="19"/>
+      <c r="Y16" s="19"/>
+      <c r="Z16" s="19"/>
     </row>
     <row r="17" spans="1:31" ht="20.25">
       <c r="A17" s="8"/>
@@ -1923,34 +1933,34 @@
       <c r="Z17" s="8"/>
     </row>
     <row r="18" spans="1:31" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
-      <c r="S18" s="13"/>
-      <c r="T18" s="13"/>
-      <c r="U18" s="13"/>
-      <c r="V18" s="13"/>
-      <c r="W18" s="13"/>
-      <c r="X18" s="13"/>
-      <c r="Y18" s="13"/>
-      <c r="Z18" s="13"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="18"/>
+      <c r="S18" s="18"/>
+      <c r="T18" s="18"/>
+      <c r="U18" s="18"/>
+      <c r="V18" s="18"/>
+      <c r="W18" s="18"/>
+      <c r="X18" s="18"/>
+      <c r="Y18" s="18"/>
+      <c r="Z18" s="18"/>
       <c r="AA18" s="2"/>
       <c r="AB18" s="2"/>
       <c r="AC18" s="2"/>
@@ -1958,34 +1968,34 @@
       <c r="AE18" s="2"/>
     </row>
     <row r="19" spans="1:31" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="13"/>
-      <c r="R19" s="13"/>
-      <c r="S19" s="13"/>
-      <c r="T19" s="13"/>
-      <c r="U19" s="13"/>
-      <c r="V19" s="13"/>
-      <c r="W19" s="13"/>
-      <c r="X19" s="13"/>
-      <c r="Y19" s="13"/>
-      <c r="Z19" s="13"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="18"/>
+      <c r="S19" s="18"/>
+      <c r="T19" s="18"/>
+      <c r="U19" s="18"/>
+      <c r="V19" s="18"/>
+      <c r="W19" s="18"/>
+      <c r="X19" s="18"/>
+      <c r="Y19" s="18"/>
+      <c r="Z19" s="18"/>
       <c r="AA19" s="2"/>
       <c r="AB19" s="2"/>
       <c r="AC19" s="2"/>
@@ -1993,34 +2003,34 @@
       <c r="AE19" s="2"/>
     </row>
     <row r="20" spans="1:31" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
-      <c r="R20" s="13"/>
-      <c r="S20" s="13"/>
-      <c r="T20" s="13"/>
-      <c r="U20" s="13"/>
-      <c r="V20" s="13"/>
-      <c r="W20" s="13"/>
-      <c r="X20" s="13"/>
-      <c r="Y20" s="13"/>
-      <c r="Z20" s="13"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="18"/>
+      <c r="T20" s="18"/>
+      <c r="U20" s="18"/>
+      <c r="V20" s="18"/>
+      <c r="W20" s="18"/>
+      <c r="X20" s="18"/>
+      <c r="Y20" s="18"/>
+      <c r="Z20" s="18"/>
       <c r="AA20" s="2"/>
       <c r="AB20" s="2"/>
       <c r="AC20" s="2"/>
@@ -2028,100 +2038,100 @@
       <c r="AE20" s="2"/>
     </row>
     <row r="21" spans="1:31" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13" t="s">
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13"/>
-      <c r="T21" s="13"/>
-      <c r="U21" s="13"/>
-      <c r="V21" s="13"/>
-      <c r="W21" s="13"/>
-      <c r="X21" s="13"/>
-      <c r="Y21" s="13"/>
-      <c r="Z21" s="13"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="18"/>
+      <c r="T21" s="18"/>
+      <c r="U21" s="18"/>
+      <c r="V21" s="18"/>
+      <c r="W21" s="18"/>
+      <c r="X21" s="18"/>
+      <c r="Y21" s="18"/>
+      <c r="Z21" s="18"/>
       <c r="AA21" s="9"/>
     </row>
     <row r="22" spans="1:31" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13" t="s">
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="13"/>
-      <c r="S22" s="13"/>
-      <c r="T22" s="13"/>
-      <c r="U22" s="13"/>
-      <c r="V22" s="13"/>
-      <c r="W22" s="13"/>
-      <c r="X22" s="13"/>
-      <c r="Y22" s="13"/>
-      <c r="Z22" s="13"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
+      <c r="S22" s="18"/>
+      <c r="T22" s="18"/>
+      <c r="U22" s="18"/>
+      <c r="V22" s="18"/>
+      <c r="W22" s="18"/>
+      <c r="X22" s="18"/>
+      <c r="Y22" s="18"/>
+      <c r="Z22" s="18"/>
       <c r="AA22" s="10"/>
     </row>
     <row r="23" spans="1:31" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="13"/>
-      <c r="S23" s="13"/>
-      <c r="T23" s="13"/>
-      <c r="U23" s="13"/>
-      <c r="V23" s="13"/>
-      <c r="W23" s="13"/>
-      <c r="X23" s="13"/>
-      <c r="Y23" s="13"/>
-      <c r="Z23" s="13"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="18"/>
+      <c r="T23" s="18"/>
+      <c r="U23" s="18"/>
+      <c r="V23" s="18"/>
+      <c r="W23" s="18"/>
+      <c r="X23" s="18"/>
+      <c r="Y23" s="18"/>
+      <c r="Z23" s="18"/>
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
       <c r="AC23" s="2"/>
@@ -2129,34 +2139,34 @@
       <c r="AE23" s="2"/>
     </row>
     <row r="24" spans="1:31" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="13"/>
-      <c r="R24" s="13"/>
-      <c r="S24" s="13"/>
-      <c r="T24" s="13"/>
-      <c r="U24" s="13"/>
-      <c r="V24" s="13"/>
-      <c r="W24" s="13"/>
-      <c r="X24" s="13"/>
-      <c r="Y24" s="13"/>
-      <c r="Z24" s="13"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="18"/>
+      <c r="T24" s="18"/>
+      <c r="U24" s="18"/>
+      <c r="V24" s="18"/>
+      <c r="W24" s="18"/>
+      <c r="X24" s="18"/>
+      <c r="Y24" s="18"/>
+      <c r="Z24" s="18"/>
       <c r="AA24" s="2"/>
       <c r="AB24" s="2"/>
       <c r="AC24" s="2"/>
@@ -2303,6 +2313,20 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A23:Z23"/>
+    <mergeCell ref="A24:Z24"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="I28:R28"/>
+    <mergeCell ref="S28:Z28"/>
+    <mergeCell ref="A22:K22"/>
+    <mergeCell ref="L22:Z22"/>
+    <mergeCell ref="A15:Z15"/>
+    <mergeCell ref="A16:Z16"/>
+    <mergeCell ref="A18:Z18"/>
+    <mergeCell ref="A19:Z19"/>
+    <mergeCell ref="A20:Z20"/>
+    <mergeCell ref="A21:K21"/>
+    <mergeCell ref="L21:Z21"/>
     <mergeCell ref="A1:Z1"/>
     <mergeCell ref="A2:Z2"/>
     <mergeCell ref="A14:H14"/>
@@ -2317,20 +2341,6 @@
     <mergeCell ref="K7:Z7"/>
     <mergeCell ref="A8:J8"/>
     <mergeCell ref="K8:Z8"/>
-    <mergeCell ref="A22:K22"/>
-    <mergeCell ref="L22:Z22"/>
-    <mergeCell ref="A15:Z15"/>
-    <mergeCell ref="A16:Z16"/>
-    <mergeCell ref="A18:Z18"/>
-    <mergeCell ref="A19:Z19"/>
-    <mergeCell ref="A20:Z20"/>
-    <mergeCell ref="A21:K21"/>
-    <mergeCell ref="L21:Z21"/>
-    <mergeCell ref="A23:Z23"/>
-    <mergeCell ref="A24:Z24"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="I28:R28"/>
-    <mergeCell ref="S28:Z28"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2356,271 +2366,297 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
+      <c r="Y1" s="20"/>
+      <c r="Z1" s="20"/>
     </row>
     <row r="3" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19" t="s">
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19" t="s">
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="R3" s="19"/>
-      <c r="S3" s="19"/>
-      <c r="T3" s="19"/>
-      <c r="U3" s="19"/>
-      <c r="V3" s="19"/>
-      <c r="W3" s="19"/>
-      <c r="X3" s="19"/>
-      <c r="Y3" s="19"/>
-      <c r="Z3" s="19"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="21"/>
+      <c r="X3" s="21"/>
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="21"/>
     </row>
     <row r="4" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19" t="s">
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19" t="s">
+      <c r="R4" s="21"/>
+      <c r="S4" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="T4" s="19"/>
-      <c r="U4" s="19" t="s">
+      <c r="T4" s="21"/>
+      <c r="U4" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="V4" s="19"/>
-      <c r="W4" s="19" t="s">
+      <c r="V4" s="21"/>
+      <c r="W4" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="X4" s="19"/>
-      <c r="Y4" s="19" t="s">
+      <c r="X4" s="21"/>
+      <c r="Y4" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="Z4" s="19"/>
+      <c r="Z4" s="21"/>
     </row>
     <row r="5" spans="1:26" ht="39.950000000000003" customHeight="1">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="19"/>
-      <c r="S5" s="19"/>
-      <c r="T5" s="19"/>
-      <c r="U5" s="19"/>
-      <c r="V5" s="19"/>
-      <c r="W5" s="19"/>
-      <c r="X5" s="19"/>
-      <c r="Y5" s="19"/>
-      <c r="Z5" s="19"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="21"/>
+      <c r="V5" s="21"/>
+      <c r="W5" s="21"/>
+      <c r="X5" s="21"/>
+      <c r="Y5" s="21"/>
+      <c r="Z5" s="21"/>
     </row>
     <row r="7" spans="1:26" ht="24.95" customHeight="1">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="22"/>
-      <c r="S7" s="22"/>
-      <c r="T7" s="22"/>
-      <c r="U7" s="22"/>
-      <c r="V7" s="22"/>
-      <c r="W7" s="22"/>
-      <c r="X7" s="22"/>
-      <c r="Y7" s="22"/>
-      <c r="Z7" s="22"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="23"/>
+      <c r="V7" s="23"/>
+      <c r="W7" s="23"/>
+      <c r="X7" s="23"/>
+      <c r="Y7" s="23"/>
+      <c r="Z7" s="23"/>
     </row>
     <row r="9" spans="1:26" ht="24.95" customHeight="1">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21" t="s">
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21" t="s">
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21" t="s">
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="21"/>
-      <c r="U9" s="21"/>
-      <c r="V9" s="21"/>
-      <c r="W9" s="21"/>
-      <c r="X9" s="21"/>
-      <c r="Y9" s="21"/>
-      <c r="Z9" s="21"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="24"/>
+      <c r="V9" s="24"/>
+      <c r="W9" s="24"/>
+      <c r="X9" s="24"/>
+      <c r="Y9" s="24"/>
+      <c r="Z9" s="24"/>
     </row>
     <row r="10" spans="1:26" ht="24.95" customHeight="1">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="19" t="s">
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="R10" s="19"/>
-      <c r="S10" s="19" t="s">
+      <c r="R10" s="21"/>
+      <c r="S10" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="T10" s="19"/>
-      <c r="U10" s="19" t="s">
+      <c r="T10" s="21"/>
+      <c r="U10" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="V10" s="19"/>
-      <c r="W10" s="19" t="s">
+      <c r="V10" s="21"/>
+      <c r="W10" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="X10" s="19"/>
-      <c r="Y10" s="19" t="s">
+      <c r="X10" s="21"/>
+      <c r="Y10" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="Z10" s="19"/>
+      <c r="Z10" s="21"/>
     </row>
     <row r="11" spans="1:26" ht="50.1" customHeight="1">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="19"/>
-      <c r="S11" s="19"/>
-      <c r="T11" s="19"/>
-      <c r="U11" s="19"/>
-      <c r="V11" s="19"/>
-      <c r="W11" s="19"/>
-      <c r="X11" s="19"/>
-      <c r="Y11" s="19"/>
-      <c r="Z11" s="19"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="21"/>
+      <c r="U11" s="21"/>
+      <c r="V11" s="21"/>
+      <c r="W11" s="21"/>
+      <c r="X11" s="21"/>
+      <c r="Y11" s="21"/>
+      <c r="Z11" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="W11:X11"/>
+    <mergeCell ref="Y11:Z11"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="L11:P11"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="S11:T11"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="A9:F10"/>
+    <mergeCell ref="G9:K10"/>
+    <mergeCell ref="L9:P10"/>
+    <mergeCell ref="Q9:Z9"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="A7:Z7"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="L3:P4"/>
+    <mergeCell ref="G3:K4"/>
+    <mergeCell ref="A3:F4"/>
     <mergeCell ref="A1:Z1"/>
     <mergeCell ref="Y5:Z5"/>
     <mergeCell ref="Q5:R5"/>
@@ -2631,32 +2667,6 @@
     <mergeCell ref="G5:K5"/>
     <mergeCell ref="L5:P5"/>
     <mergeCell ref="Q3:Z3"/>
-    <mergeCell ref="A7:Z7"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="L3:P4"/>
-    <mergeCell ref="G3:K4"/>
-    <mergeCell ref="A3:F4"/>
-    <mergeCell ref="A9:F10"/>
-    <mergeCell ref="G9:K10"/>
-    <mergeCell ref="L9:P10"/>
-    <mergeCell ref="Q9:Z9"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="W11:X11"/>
-    <mergeCell ref="Y11:Z11"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="L11:P11"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="S11:T11"/>
-    <mergeCell ref="U11:V11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="88" orientation="landscape" r:id="rId1"/>
@@ -2670,8 +2680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F026DA5C-28E1-47C4-AC05-B4794F49A0ED}">
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:Z7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -2681,281 +2691,281 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
+      <c r="Y1" s="20"/>
+      <c r="Z1" s="20"/>
     </row>
     <row r="3" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19" t="s">
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19" t="s">
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="R3" s="19"/>
-      <c r="S3" s="19"/>
-      <c r="T3" s="19"/>
-      <c r="U3" s="19"/>
-      <c r="V3" s="19"/>
-      <c r="W3" s="19"/>
-      <c r="X3" s="19"/>
-      <c r="Y3" s="19"/>
-      <c r="Z3" s="19"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="21"/>
+      <c r="X3" s="21"/>
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="21"/>
     </row>
     <row r="4" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19" t="s">
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19" t="s">
+      <c r="R4" s="21"/>
+      <c r="S4" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="T4" s="19"/>
-      <c r="U4" s="19" t="s">
+      <c r="T4" s="21"/>
+      <c r="U4" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="V4" s="19"/>
-      <c r="W4" s="19" t="s">
+      <c r="V4" s="21"/>
+      <c r="W4" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="X4" s="19"/>
-      <c r="Y4" s="19" t="s">
+      <c r="X4" s="21"/>
+      <c r="Y4" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="Z4" s="19"/>
+      <c r="Z4" s="21"/>
     </row>
     <row r="5" spans="1:26" ht="39.950000000000003" customHeight="1">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="19"/>
-      <c r="S5" s="19"/>
-      <c r="T5" s="19"/>
-      <c r="U5" s="19"/>
-      <c r="V5" s="19"/>
-      <c r="W5" s="19"/>
-      <c r="X5" s="19"/>
-      <c r="Y5" s="19"/>
-      <c r="Z5" s="19"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="21"/>
+      <c r="V5" s="21"/>
+      <c r="W5" s="21"/>
+      <c r="X5" s="21"/>
+      <c r="Y5" s="21"/>
+      <c r="Z5" s="21"/>
     </row>
     <row r="7" spans="1:26" ht="24.95" customHeight="1">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="22"/>
-      <c r="S7" s="22"/>
-      <c r="T7" s="22"/>
-      <c r="U7" s="22"/>
-      <c r="V7" s="22"/>
-      <c r="W7" s="22"/>
-      <c r="X7" s="22"/>
-      <c r="Y7" s="22"/>
-      <c r="Z7" s="22"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="23"/>
+      <c r="V7" s="23"/>
+      <c r="W7" s="23"/>
+      <c r="X7" s="23"/>
+      <c r="Y7" s="23"/>
+      <c r="Z7" s="23"/>
     </row>
     <row r="9" spans="1:26" ht="24.95" customHeight="1">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21" t="s">
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21" t="s">
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21" t="s">
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="21"/>
-      <c r="U9" s="21"/>
-      <c r="V9" s="21"/>
-      <c r="W9" s="21"/>
-      <c r="X9" s="21"/>
-      <c r="Y9" s="21"/>
-      <c r="Z9" s="21"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="24"/>
+      <c r="V9" s="24"/>
+      <c r="W9" s="24"/>
+      <c r="X9" s="24"/>
+      <c r="Y9" s="24"/>
+      <c r="Z9" s="24"/>
     </row>
     <row r="10" spans="1:26" ht="24.95" customHeight="1">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="19" t="s">
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="R10" s="19"/>
-      <c r="S10" s="19" t="s">
+      <c r="R10" s="21"/>
+      <c r="S10" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="T10" s="19"/>
-      <c r="U10" s="19" t="s">
+      <c r="T10" s="21"/>
+      <c r="U10" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="V10" s="19"/>
-      <c r="W10" s="19" t="s">
+      <c r="V10" s="21"/>
+      <c r="W10" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="X10" s="19"/>
-      <c r="Y10" s="19" t="s">
+      <c r="X10" s="21"/>
+      <c r="Y10" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="Z10" s="19"/>
+      <c r="Z10" s="21"/>
     </row>
     <row r="11" spans="1:26" ht="50.1" customHeight="1">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="19"/>
-      <c r="S11" s="19"/>
-      <c r="T11" s="19"/>
-      <c r="U11" s="19"/>
-      <c r="V11" s="19"/>
-      <c r="W11" s="19"/>
-      <c r="X11" s="19"/>
-      <c r="Y11" s="19"/>
-      <c r="Z11" s="19"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="21"/>
+      <c r="U11" s="21"/>
+      <c r="V11" s="21"/>
+      <c r="W11" s="21"/>
+      <c r="X11" s="21"/>
+      <c r="Y11" s="21"/>
+      <c r="Z11" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="L11:P11"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="S11:T11"/>
-    <mergeCell ref="U11:V11"/>
-    <mergeCell ref="W11:X11"/>
-    <mergeCell ref="Y11:Z11"/>
+    <mergeCell ref="A1:Z1"/>
+    <mergeCell ref="A3:F4"/>
+    <mergeCell ref="G3:K4"/>
+    <mergeCell ref="L3:P4"/>
+    <mergeCell ref="Q3:Z3"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="Y4:Z4"/>
     <mergeCell ref="W5:X5"/>
     <mergeCell ref="Y5:Z5"/>
     <mergeCell ref="A7:Z7"/>
@@ -2972,16 +2982,16 @@
     <mergeCell ref="Q5:R5"/>
     <mergeCell ref="S5:T5"/>
     <mergeCell ref="U5:V5"/>
-    <mergeCell ref="A1:Z1"/>
-    <mergeCell ref="A3:F4"/>
-    <mergeCell ref="G3:K4"/>
-    <mergeCell ref="L3:P4"/>
-    <mergeCell ref="Q3:Z3"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="W10:X10"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="L11:P11"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="S11:T11"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="W11:X11"/>
+    <mergeCell ref="Y11:Z11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="88" orientation="landscape" r:id="rId1"/>
@@ -2996,264 +3006,1014 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AD30"/>
+  <dimension ref="A1:AD34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AF8" sqref="AF8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="14" width="5.7109375" style="12" customWidth="1"/>
     <col min="15" max="26" width="4.42578125" style="12" customWidth="1"/>
-    <col min="27" max="30" width="4.42578125" style="25" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="25"/>
+    <col min="27" max="30" width="4.42578125" style="13" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="20.100000000000001" customHeight="1">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-      <c r="AB1" s="23"/>
-      <c r="AC1" s="23"/>
-      <c r="AD1" s="23"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
+      <c r="Y1" s="20"/>
+      <c r="Z1" s="20"/>
+      <c r="AA1" s="20"/>
+      <c r="AB1" s="20"/>
+      <c r="AC1" s="20"/>
+      <c r="AD1" s="20"/>
     </row>
     <row r="2" spans="1:30" ht="20.100000000000001" customHeight="1"/>
     <row r="3" spans="1:30" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19" t="s">
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="19"/>
-      <c r="S3" s="19" t="s">
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="T3" s="19"/>
-      <c r="U3" s="19"/>
-      <c r="V3" s="19"/>
-      <c r="W3" s="19" t="s">
+      <c r="T3" s="21"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="X3" s="19"/>
-      <c r="Y3" s="19"/>
-      <c r="Z3" s="19"/>
-      <c r="AA3" s="19" t="s">
+      <c r="X3" s="21"/>
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="21"/>
+      <c r="AA3" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="AB3" s="19"/>
-      <c r="AC3" s="19"/>
-      <c r="AD3" s="19"/>
+      <c r="AB3" s="21"/>
+      <c r="AC3" s="21"/>
+      <c r="AD3" s="21"/>
     </row>
     <row r="4" spans="1:30" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="27"/>
-      <c r="S4" s="27"/>
-      <c r="T4" s="27"/>
-      <c r="U4" s="27"/>
-      <c r="V4" s="27"/>
-      <c r="W4" s="27"/>
-      <c r="X4" s="27"/>
-      <c r="Y4" s="27"/>
-      <c r="Z4" s="27"/>
-      <c r="AA4" s="27"/>
-      <c r="AB4" s="27"/>
-      <c r="AC4" s="27"/>
-      <c r="AD4" s="27"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="26"/>
+      <c r="V4" s="26"/>
+      <c r="W4" s="26"/>
+      <c r="X4" s="26"/>
+      <c r="Y4" s="26"/>
+      <c r="Z4" s="26"/>
+      <c r="AA4" s="26"/>
+      <c r="AB4" s="26"/>
+      <c r="AC4" s="26"/>
+      <c r="AD4" s="26"/>
     </row>
     <row r="5" spans="1:30" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="21"/>
+      <c r="V5" s="21"/>
+      <c r="W5" s="21"/>
+      <c r="X5" s="21"/>
+      <c r="Y5" s="21"/>
+      <c r="Z5" s="21"/>
+      <c r="AA5" s="21"/>
+      <c r="AB5" s="21"/>
+      <c r="AC5" s="21"/>
+      <c r="AD5" s="21"/>
+    </row>
+    <row r="6" spans="1:30" ht="20.100000000000001" customHeight="1">
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21">
+        <f>SUM($O$4:O5)</f>
+        <v>0</v>
+      </c>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="21"/>
+      <c r="S6" s="21">
+        <f>SUM($S$4:S5)</f>
+        <v>0</v>
+      </c>
+      <c r="T6" s="21"/>
+      <c r="U6" s="21"/>
+      <c r="V6" s="21"/>
+      <c r="W6" s="21">
+        <f>SUM($W$4:W5)</f>
+        <v>0</v>
+      </c>
+      <c r="X6" s="21"/>
+      <c r="Y6" s="21"/>
+      <c r="Z6" s="21"/>
+      <c r="AA6" s="21">
+        <f>SUM($AA$4:AA5)</f>
+        <v>0</v>
+      </c>
+      <c r="AB6" s="21"/>
+      <c r="AC6" s="21"/>
+      <c r="AD6" s="21"/>
+    </row>
+    <row r="7" spans="1:30" ht="20.100000000000001" customHeight="1">
+      <c r="A7" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="27"/>
-      <c r="S5" s="27"/>
-      <c r="T5" s="27"/>
-      <c r="U5" s="27"/>
-      <c r="V5" s="27"/>
-      <c r="W5" s="27"/>
-      <c r="X5" s="27"/>
-      <c r="Y5" s="27"/>
-      <c r="Z5" s="27"/>
-      <c r="AA5" s="27"/>
-      <c r="AB5" s="27"/>
-      <c r="AC5" s="27"/>
-      <c r="AD5" s="27"/>
-    </row>
-    <row r="6" spans="1:30" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="26" t="s">
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="26"/>
+      <c r="S7" s="26"/>
+      <c r="T7" s="26"/>
+      <c r="U7" s="26"/>
+      <c r="V7" s="26"/>
+      <c r="W7" s="26"/>
+      <c r="X7" s="26"/>
+      <c r="Y7" s="26"/>
+      <c r="Z7" s="26"/>
+      <c r="AA7" s="26"/>
+      <c r="AB7" s="26"/>
+      <c r="AC7" s="26"/>
+      <c r="AD7" s="26"/>
+    </row>
+    <row r="8" spans="1:30" ht="20.100000000000001" customHeight="1">
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
+      <c r="S8" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="T8" s="21"/>
+      <c r="U8" s="21"/>
+      <c r="V8" s="21"/>
+      <c r="W8" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="X8" s="21"/>
+      <c r="Y8" s="21"/>
+      <c r="Z8" s="21"/>
+      <c r="AA8" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB8" s="21"/>
+      <c r="AC8" s="21"/>
+      <c r="AD8" s="21"/>
+    </row>
+    <row r="9" spans="1:30" ht="20.100000000000001" customHeight="1">
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21">
+        <f>SUM($O$7:O8)</f>
+        <v>0</v>
+      </c>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="21">
+        <f>SUM($S$7:S8)</f>
+        <v>0</v>
+      </c>
+      <c r="T9" s="21"/>
+      <c r="U9" s="21"/>
+      <c r="V9" s="21"/>
+      <c r="W9" s="21">
+        <f>SUM($W$7:W8)</f>
+        <v>0</v>
+      </c>
+      <c r="X9" s="21"/>
+      <c r="Y9" s="21"/>
+      <c r="Z9" s="21"/>
+      <c r="AA9" s="21">
+        <f>SUM($AA$7:AA8)</f>
+        <v>0</v>
+      </c>
+      <c r="AB9" s="21"/>
+      <c r="AC9" s="21"/>
+      <c r="AD9" s="21"/>
+    </row>
+    <row r="10" spans="1:30" ht="20.100000000000001" customHeight="1">
+      <c r="A10" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="28" t="s">
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="28" t="s">
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="R6" s="29"/>
-      <c r="S6" s="28" t="s">
+      <c r="R10" s="21"/>
+      <c r="S10" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="T6" s="29"/>
-      <c r="U6" s="28" t="s">
+      <c r="T10" s="21"/>
+      <c r="U10" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="V6" s="29"/>
-      <c r="W6" s="28" t="s">
+      <c r="V10" s="21"/>
+      <c r="W10" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="X6" s="29"/>
-      <c r="Y6" s="28" t="s">
+      <c r="X10" s="21"/>
+      <c r="Y10" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="Z6" s="29"/>
-      <c r="AA6" s="28" t="s">
+      <c r="Z10" s="21"/>
+      <c r="AA10" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="AB6" s="29"/>
-      <c r="AC6" s="28" t="s">
+      <c r="AB10" s="21"/>
+      <c r="AC10" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="AD6" s="29"/>
-    </row>
-    <row r="7" spans="1:30" ht="20.100000000000001" customHeight="1"/>
-    <row r="8" spans="1:30" ht="20.100000000000001" customHeight="1"/>
-    <row r="9" spans="1:30" ht="20.100000000000001" customHeight="1"/>
-    <row r="10" spans="1:30" ht="20.100000000000001" customHeight="1"/>
-    <row r="11" spans="1:30" ht="20.100000000000001" customHeight="1"/>
-    <row r="12" spans="1:30" ht="20.100000000000001" customHeight="1"/>
+      <c r="AD10" s="21"/>
+    </row>
+    <row r="11" spans="1:30" ht="20.100000000000001" customHeight="1">
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="21"/>
+      <c r="U11" s="21"/>
+      <c r="V11" s="21"/>
+      <c r="W11" s="21"/>
+      <c r="X11" s="21"/>
+      <c r="Y11" s="21"/>
+      <c r="Z11" s="21"/>
+      <c r="AA11" s="21"/>
+      <c r="AB11" s="21"/>
+      <c r="AC11" s="21"/>
+      <c r="AD11" s="21"/>
+    </row>
+    <row r="12" spans="1:30" ht="20.100000000000001" customHeight="1">
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="21"/>
+      <c r="T12" s="21"/>
+      <c r="U12" s="21"/>
+      <c r="V12" s="21"/>
+      <c r="W12" s="21"/>
+      <c r="X12" s="21"/>
+      <c r="Y12" s="21"/>
+      <c r="Z12" s="21"/>
+      <c r="AA12" s="21"/>
+      <c r="AB12" s="21"/>
+      <c r="AC12" s="21"/>
+      <c r="AD12" s="21"/>
+    </row>
     <row r="13" spans="1:30" ht="20.100000000000001" customHeight="1"/>
-    <row r="14" spans="1:30" ht="20.100000000000001" customHeight="1"/>
+    <row r="14" spans="1:30" ht="20.100000000000001" customHeight="1">
+      <c r="A14" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="20"/>
+      <c r="U14" s="20"/>
+      <c r="V14" s="20"/>
+      <c r="W14" s="20"/>
+      <c r="X14" s="20"/>
+      <c r="Y14" s="20"/>
+      <c r="Z14" s="20"/>
+      <c r="AA14" s="20"/>
+      <c r="AB14" s="20"/>
+      <c r="AC14" s="20"/>
+      <c r="AD14" s="20"/>
+    </row>
     <row r="15" spans="1:30" ht="20.100000000000001" customHeight="1"/>
-    <row r="16" spans="1:30" ht="20.100000000000001" customHeight="1"/>
-    <row r="17" ht="20.100000000000001" customHeight="1"/>
-    <row r="18" ht="20.100000000000001" customHeight="1"/>
-    <row r="19" ht="20.100000000000001" customHeight="1"/>
-    <row r="20" ht="20.100000000000001" customHeight="1"/>
-    <row r="21" ht="20.100000000000001" customHeight="1"/>
-    <row r="22" ht="20.100000000000001" customHeight="1"/>
-    <row r="23" ht="20.100000000000001" customHeight="1"/>
-    <row r="24" ht="20.100000000000001" customHeight="1"/>
-    <row r="25" ht="20.100000000000001" customHeight="1"/>
-    <row r="26" ht="20.100000000000001" customHeight="1"/>
-    <row r="27" ht="20.100000000000001" customHeight="1"/>
-    <row r="28" ht="20.100000000000001" customHeight="1"/>
-    <row r="29" ht="20.100000000000001" customHeight="1"/>
-    <row r="30" ht="20.100000000000001" customHeight="1"/>
+    <row r="16" spans="1:30" ht="20.100000000000001" customHeight="1">
+      <c r="A16" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="21"/>
+      <c r="R16" s="21"/>
+      <c r="S16" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="T16" s="21"/>
+      <c r="U16" s="21"/>
+      <c r="V16" s="21"/>
+      <c r="W16" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="X16" s="21"/>
+      <c r="Y16" s="21"/>
+      <c r="Z16" s="21"/>
+      <c r="AA16" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB16" s="21"/>
+      <c r="AC16" s="21"/>
+      <c r="AD16" s="21"/>
+    </row>
+    <row r="17" spans="1:30" ht="20.100000000000001" customHeight="1">
+      <c r="A17" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="26"/>
+      <c r="R17" s="26"/>
+      <c r="S17" s="26"/>
+      <c r="T17" s="26"/>
+      <c r="U17" s="26"/>
+      <c r="V17" s="26"/>
+      <c r="W17" s="26"/>
+      <c r="X17" s="26"/>
+      <c r="Y17" s="26"/>
+      <c r="Z17" s="26"/>
+      <c r="AA17" s="26"/>
+      <c r="AB17" s="26"/>
+      <c r="AC17" s="26"/>
+      <c r="AD17" s="26"/>
+    </row>
+    <row r="18" spans="1:30" ht="20.100000000000001" customHeight="1">
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="26"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="21"/>
+      <c r="U18" s="21"/>
+      <c r="V18" s="21"/>
+      <c r="W18" s="21"/>
+      <c r="X18" s="21"/>
+      <c r="Y18" s="21"/>
+      <c r="Z18" s="21"/>
+      <c r="AA18" s="21"/>
+      <c r="AB18" s="21"/>
+      <c r="AC18" s="21"/>
+      <c r="AD18" s="21"/>
+    </row>
+    <row r="19" spans="1:30" ht="20.100000000000001" customHeight="1">
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="21">
+        <f>SUM($O$17:O18)</f>
+        <v>0</v>
+      </c>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="21">
+        <f>SUM($S$17:S18)</f>
+        <v>0</v>
+      </c>
+      <c r="T19" s="21"/>
+      <c r="U19" s="21"/>
+      <c r="V19" s="21"/>
+      <c r="W19" s="21">
+        <f>SUM($W$17:W18)</f>
+        <v>0</v>
+      </c>
+      <c r="X19" s="21"/>
+      <c r="Y19" s="21"/>
+      <c r="Z19" s="21"/>
+      <c r="AA19" s="21">
+        <f>SUM($AA$17:AA18)</f>
+        <v>0</v>
+      </c>
+      <c r="AB19" s="21"/>
+      <c r="AC19" s="21"/>
+      <c r="AD19" s="21"/>
+    </row>
+    <row r="20" spans="1:30" ht="20.100000000000001" customHeight="1">
+      <c r="A20" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="26"/>
+      <c r="O20" s="26"/>
+      <c r="P20" s="26"/>
+      <c r="Q20" s="26"/>
+      <c r="R20" s="26"/>
+      <c r="S20" s="26"/>
+      <c r="T20" s="26"/>
+      <c r="U20" s="26"/>
+      <c r="V20" s="26"/>
+      <c r="W20" s="26"/>
+      <c r="X20" s="26"/>
+      <c r="Y20" s="26"/>
+      <c r="Z20" s="26"/>
+      <c r="AA20" s="26"/>
+      <c r="AB20" s="26"/>
+      <c r="AC20" s="26"/>
+      <c r="AD20" s="26"/>
+    </row>
+    <row r="21" spans="1:30" ht="20.100000000000001" customHeight="1">
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="21"/>
+      <c r="Q21" s="21"/>
+      <c r="R21" s="21"/>
+      <c r="S21" s="21"/>
+      <c r="T21" s="21"/>
+      <c r="U21" s="21"/>
+      <c r="V21" s="21"/>
+      <c r="W21" s="21"/>
+      <c r="X21" s="21"/>
+      <c r="Y21" s="21"/>
+      <c r="Z21" s="21"/>
+      <c r="AA21" s="21"/>
+      <c r="AB21" s="21"/>
+      <c r="AC21" s="21"/>
+      <c r="AD21" s="21"/>
+    </row>
+    <row r="22" spans="1:30" ht="20.100000000000001" customHeight="1">
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="21">
+        <f>SUM($O$20:O21)</f>
+        <v>0</v>
+      </c>
+      <c r="P22" s="21"/>
+      <c r="Q22" s="21"/>
+      <c r="R22" s="21"/>
+      <c r="S22" s="21">
+        <f>SUM($S$20:S21)</f>
+        <v>0</v>
+      </c>
+      <c r="T22" s="21"/>
+      <c r="U22" s="21"/>
+      <c r="V22" s="21"/>
+      <c r="W22" s="21">
+        <f>SUM($W$20:W21)</f>
+        <v>0</v>
+      </c>
+      <c r="X22" s="21"/>
+      <c r="Y22" s="21"/>
+      <c r="Z22" s="21"/>
+      <c r="AA22" s="21">
+        <f>SUM($AA$20:AA21)</f>
+        <v>0</v>
+      </c>
+      <c r="AB22" s="21"/>
+      <c r="AC22" s="21"/>
+      <c r="AD22" s="21"/>
+    </row>
+    <row r="23" spans="1:30" ht="20.100000000000001" customHeight="1">
+      <c r="A23" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="26"/>
+      <c r="N23" s="26"/>
+      <c r="O23" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="P23" s="21"/>
+      <c r="Q23" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="R23" s="21"/>
+      <c r="S23" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="T23" s="21"/>
+      <c r="U23" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="V23" s="21"/>
+      <c r="W23" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="X23" s="21"/>
+      <c r="Y23" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z23" s="21"/>
+      <c r="AA23" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB23" s="21"/>
+      <c r="AC23" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD23" s="21"/>
+    </row>
+    <row r="24" spans="1:30" ht="20.100000000000001" customHeight="1">
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="21"/>
+      <c r="Q24" s="21"/>
+      <c r="R24" s="21"/>
+      <c r="S24" s="21"/>
+      <c r="T24" s="21"/>
+      <c r="U24" s="21"/>
+      <c r="V24" s="21"/>
+      <c r="W24" s="21"/>
+      <c r="X24" s="21"/>
+      <c r="Y24" s="21"/>
+      <c r="Z24" s="21"/>
+      <c r="AA24" s="21"/>
+      <c r="AB24" s="21"/>
+      <c r="AC24" s="21"/>
+      <c r="AD24" s="21"/>
+    </row>
+    <row r="25" spans="1:30" ht="20.100000000000001" customHeight="1">
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="21"/>
+      <c r="R25" s="21"/>
+      <c r="S25" s="21"/>
+      <c r="T25" s="21"/>
+      <c r="U25" s="21"/>
+      <c r="V25" s="21"/>
+      <c r="W25" s="21"/>
+      <c r="X25" s="21"/>
+      <c r="Y25" s="21"/>
+      <c r="Z25" s="21"/>
+      <c r="AA25" s="21"/>
+      <c r="AB25" s="21"/>
+      <c r="AC25" s="21"/>
+      <c r="AD25" s="21"/>
+    </row>
+    <row r="26" spans="1:30" ht="20.100000000000001" customHeight="1"/>
+    <row r="27" spans="1:30" ht="20.100000000000001" customHeight="1"/>
+    <row r="28" spans="1:30" ht="20.100000000000001" customHeight="1"/>
+    <row r="29" spans="1:30" ht="20.100000000000001" customHeight="1"/>
+    <row r="30" spans="1:30" ht="20.100000000000001" customHeight="1"/>
+    <row r="31" spans="1:30" ht="20.100000000000001" customHeight="1"/>
+    <row r="32" spans="1:30" ht="20.100000000000001" customHeight="1"/>
+    <row r="33" ht="20.100000000000001" customHeight="1"/>
+    <row r="34" ht="20.100000000000001" customHeight="1"/>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="A6:N6"/>
-    <mergeCell ref="W3:Z3"/>
-    <mergeCell ref="AA3:AD3"/>
+  <mergeCells count="124">
+    <mergeCell ref="U25:V25"/>
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="Y25:Z25"/>
+    <mergeCell ref="AA25:AB25"/>
+    <mergeCell ref="AC25:AD25"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D25:N25"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="S25:T25"/>
+    <mergeCell ref="U24:V24"/>
+    <mergeCell ref="W24:X24"/>
+    <mergeCell ref="Y24:Z24"/>
+    <mergeCell ref="AA24:AB24"/>
+    <mergeCell ref="AC24:AD24"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="D24:N24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="AA22:AD22"/>
+    <mergeCell ref="A23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="W23:X23"/>
+    <mergeCell ref="Y23:Z23"/>
+    <mergeCell ref="AA23:AB23"/>
+    <mergeCell ref="AC23:AD23"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D22:N22"/>
+    <mergeCell ref="O22:R22"/>
+    <mergeCell ref="S22:V22"/>
+    <mergeCell ref="W22:Z22"/>
+    <mergeCell ref="AA19:AD19"/>
+    <mergeCell ref="A20:AD20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:N21"/>
+    <mergeCell ref="O21:R21"/>
+    <mergeCell ref="S21:V21"/>
+    <mergeCell ref="W21:Z21"/>
+    <mergeCell ref="AA21:AD21"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D19:N19"/>
+    <mergeCell ref="O19:R19"/>
+    <mergeCell ref="S19:V19"/>
+    <mergeCell ref="W19:Z19"/>
+    <mergeCell ref="A17:AD17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:N18"/>
+    <mergeCell ref="O18:R18"/>
+    <mergeCell ref="S18:V18"/>
+    <mergeCell ref="W18:Z18"/>
+    <mergeCell ref="AA18:AD18"/>
+    <mergeCell ref="A14:AD14"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:N16"/>
+    <mergeCell ref="O16:R16"/>
+    <mergeCell ref="S16:V16"/>
+    <mergeCell ref="W16:Z16"/>
+    <mergeCell ref="AA16:AD16"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="W12:X12"/>
+    <mergeCell ref="Y12:Z12"/>
+    <mergeCell ref="AA12:AB12"/>
+    <mergeCell ref="AC12:AD12"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="D12:N12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="W11:X11"/>
+    <mergeCell ref="Y11:Z11"/>
+    <mergeCell ref="AA11:AB11"/>
+    <mergeCell ref="AC11:AD11"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D11:N11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="S11:T11"/>
     <mergeCell ref="A1:AD1"/>
     <mergeCell ref="A4:AD4"/>
-    <mergeCell ref="A5:AD5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="A7:AD7"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
     <mergeCell ref="D3:N3"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="O3:R3"/>
     <mergeCell ref="S3:V3"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:N6"/>
+    <mergeCell ref="O6:R6"/>
+    <mergeCell ref="S6:V6"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="AC10:AD10"/>
+    <mergeCell ref="A10:N10"/>
+    <mergeCell ref="W3:Z3"/>
+    <mergeCell ref="AA3:AD3"/>
+    <mergeCell ref="W6:Z6"/>
+    <mergeCell ref="AA6:AD6"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:N9"/>
+    <mergeCell ref="O9:R9"/>
+    <mergeCell ref="S9:V9"/>
+    <mergeCell ref="W9:Z9"/>
+    <mergeCell ref="AA9:AD9"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:N5"/>
+    <mergeCell ref="O5:R5"/>
+    <mergeCell ref="S5:V5"/>
+    <mergeCell ref="W5:Z5"/>
+    <mergeCell ref="AA5:AD5"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:N8"/>
+    <mergeCell ref="O8:R8"/>
+    <mergeCell ref="S8:V8"/>
+    <mergeCell ref="W8:Z8"/>
+    <mergeCell ref="AA8:AD8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="86" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="13" max="16383" man="1"/>
+  </rowBreaks>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
[308] xóa công thức, dán giá trị
</commit_message>
<xml_diff>
--- a/KnowledgeSystem/AppResources/308_Statistic.xlsx
+++ b/KnowledgeSystem/AppResources/308_Statistic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01. Softwares Programming\24. Knowledge System\01. Projects\KnowledgeSystem\KnowledgeSystem\AppResources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDF59D6-7780-4B5D-B551-F87C74AC39CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4DE773-050F-430B-9D2E-EA7C43ECDF4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="647" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="212">
   <si>
     <t>Tên cơ sở lao động: Phòng thử nghiệm Vật lý - Bộ phận Kĩ thuật luyện kim - Công ty TNHH Gang Thép Hưng Nghiệp Formosa Hà Tĩnh</t>
   </si>
@@ -1102,31 +1102,10 @@
     <t>ĐƠN VỊ: PHÒNG THỬ NGHIỆM VẬT LÍ</t>
   </si>
   <si>
-    <t>CẬP NHẬT:26/08/2024</t>
-  </si>
-  <si>
-    <t>Nguyên nhân chưa khám sức khỏe:
-(1) Nghỉ việc 0 (H)
-(2) Không tại chức:1(G)
-(3) Thời gian chưa điều chuyển: 0 (I)
-(4) Về đài: 0 (J)
-(5) Khác: 0 (K)</t>
-  </si>
-  <si>
-    <t>Phương án xử lí
-(1) Không thể khám bù:1 (H+G)
-(2) Có thê khám bù: 0 (I+J+K)</t>
-  </si>
-  <si>
     <t>Thực tế số lượng chưa khám sức khỏe:
  - Khám đặc biệt: 0</t>
   </si>
   <si>
-    <t>Số lượng khám nửa cuối năm:
-Khám thường: 0
-Khám đặc biệt: 2</t>
-  </si>
-  <si>
     <t>Số lượng người chưa kiểm tra sức khỏe</t>
   </si>
   <si>
@@ -1178,27 +1157,6 @@
   </si>
   <si>
     <t>單位: 物理試驗處</t>
-  </si>
-  <si>
-    <t>更新日期:2024/07/08</t>
-  </si>
-  <si>
-    <t>應健檢而未健檢原因分析：
-（1）離職 0（H）
-（2）未在職：1（G)
-（3）未調換時間：0（I)
-（4）返台：0（J)
-（5）其他：0（K)</t>
-  </si>
-  <si>
-    <t>下半年應健檢人數：
-一般健檢：0
-特殊健檢：2</t>
-  </si>
-  <si>
-    <t>應健檢而未檢查處理
-（1）不可補檢：1 (H+G)
-（2）可補檢：0 (I+J+K)</t>
   </si>
   <si>
     <t>實際健檢人數： 特殊健檢：0 人</t>
@@ -1383,6 +1341,16 @@
   </si>
   <si>
     <t>K</t>
+  </si>
+  <si>
+    <t>Số lượng khám nửa cuối năm:
+Khám thường: 0
+Khám đặc biệt: 0</t>
+  </si>
+  <si>
+    <t>下半年應健檢人數：
+一般健檢：0
+特殊健檢：0</t>
   </si>
 </sst>
 </file>
@@ -3275,7 +3243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB54A37-6A6B-440D-B8CE-F296AFA571AF}">
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -3600,8 +3568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F026DA5C-28E1-47C4-AC05-B4794F49A0ED}">
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -3929,7 +3897,7 @@
   <dimension ref="A1:AD34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z2" sqref="O2:Z2"/>
+      <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -4945,7 +4913,7 @@
   <dimension ref="A1:AJ46"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AM29" sqref="AM29"/>
+      <selection activeCell="AK3" sqref="AK3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -4957,7 +4925,7 @@
   <sheetData>
     <row r="1" spans="1:36">
       <c r="A1" s="50" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -5117,13 +5085,13 @@
     </row>
     <row r="5" spans="1:36">
       <c r="A5" s="34" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
       <c r="E5" s="34" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="F5" s="34"/>
       <c r="G5" s="34"/>
@@ -5143,7 +5111,7 @@
       <c r="S5" s="34"/>
       <c r="T5" s="34"/>
       <c r="U5" s="34" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="V5" s="34"/>
       <c r="W5" s="34"/>
@@ -5165,75 +5133,75 @@
     </row>
     <row r="6" spans="1:36" ht="81.75" customHeight="1">
       <c r="A6" s="39" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="B6" s="39"/>
       <c r="C6" s="39" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="D6" s="39"/>
       <c r="E6" s="39" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="F6" s="39"/>
       <c r="G6" s="39" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="H6" s="39"/>
       <c r="I6" s="39" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="J6" s="39"/>
       <c r="K6" s="39" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="L6" s="39"/>
       <c r="M6" s="39" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="N6" s="39"/>
       <c r="O6" s="39" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="P6" s="39"/>
       <c r="Q6" s="39" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="R6" s="39"/>
       <c r="S6" s="39" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="T6" s="39"/>
       <c r="U6" s="39" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="V6" s="39"/>
       <c r="W6" s="39" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="X6" s="39"/>
       <c r="Y6" s="39" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="Z6" s="39"/>
       <c r="AA6" s="39" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="AB6" s="39"/>
       <c r="AC6" s="39" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="AD6" s="39"/>
       <c r="AE6" s="39" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="AF6" s="39"/>
       <c r="AG6" s="39" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="AH6" s="39"/>
       <c r="AI6" s="39" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="AJ6" s="39"/>
     </row>
@@ -5241,77 +5209,77 @@
       <c r="A7" s="39"/>
       <c r="B7" s="39"/>
       <c r="C7" s="44" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="D7" s="39"/>
       <c r="E7" s="44" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="F7" s="39"/>
       <c r="G7" s="44" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="H7" s="39"/>
       <c r="I7" s="44" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="J7" s="39"/>
       <c r="K7" s="44" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="L7" s="39"/>
       <c r="M7" s="44" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="N7" s="39"/>
       <c r="O7" s="44" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="P7" s="39"/>
       <c r="Q7" s="44" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="R7" s="39"/>
       <c r="S7" s="44" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="T7" s="39"/>
       <c r="U7" s="44" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="V7" s="39"/>
       <c r="W7" s="44" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="X7" s="39"/>
       <c r="Y7" s="44" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="Z7" s="39"/>
       <c r="AA7" s="44" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="AB7" s="39"/>
       <c r="AC7" s="44" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="AD7" s="39"/>
       <c r="AE7" s="44" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="AF7" s="39"/>
       <c r="AG7" s="44" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="AH7" s="39"/>
       <c r="AI7" s="44" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="AJ7" s="39"/>
     </row>
     <row r="8" spans="1:36">
       <c r="A8" s="39" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B8" s="39"/>
       <c r="C8" s="46">
@@ -5547,7 +5515,7 @@
     </row>
     <row r="11" spans="1:36">
       <c r="A11" s="39" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B11" s="39"/>
       <c r="C11" s="46">
@@ -5783,7 +5751,7 @@
     </row>
     <row r="14" spans="1:36">
       <c r="A14" s="39" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B14" s="39"/>
       <c r="C14" s="46">
@@ -6019,7 +5987,7 @@
     </row>
     <row r="17" spans="1:36">
       <c r="A17" s="39" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B17" s="39"/>
       <c r="C17" s="46">
@@ -6343,7 +6311,7 @@
     </row>
     <row r="22" spans="1:36">
       <c r="A22" s="45" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B22" s="45"/>
       <c r="C22" s="45"/>
@@ -6383,7 +6351,7 @@
     </row>
     <row r="23" spans="1:36" s="26" customFormat="1" ht="81" customHeight="1">
       <c r="A23" s="42" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B23" s="43"/>
       <c r="C23" s="43"/>
@@ -6423,7 +6391,7 @@
     </row>
     <row r="24" spans="1:36">
       <c r="A24" s="50" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B24" s="38"/>
       <c r="C24" s="38"/>
@@ -6501,8 +6469,8 @@
     </row>
     <row r="26" spans="1:36">
       <c r="A26" s="51" t="str">
-        <f ca="1">CONCATENATE("1. 休假由生病人次:","37","次(截至日期",TEXT(TODAY(),"yyyy/MM/dd"),")")</f>
-        <v>1. 休假由生病人次:37次(截至日期2025/03/10)</v>
+        <f ca="1">CONCATENATE("1. 休假由生病人次:",E20,"次(截至日期",TEXT(TODAY(),"yyyy/MM/dd"),")")</f>
+        <v>1. 休假由生病人次:0次(截至日期2025/03/10)</v>
       </c>
       <c r="B26" s="51"/>
       <c r="C26" s="51"/>
@@ -6542,7 +6510,7 @@
     </row>
     <row r="27" spans="1:36">
       <c r="A27" s="51" t="str">
-        <f ca="1">CONCATENATE("2. 休假由生病天數:",TEXT(I43,"#.##"),"天(截至日期",TEXT(TODAY(),"yyyy/MM/dd"),")")</f>
+        <f ca="1">CONCATENATE("2. 休假由生病天數:",TEXT(I20,"#.##"),"天(截至日期",TEXT(TODAY(),"yyyy/MM/dd"),")")</f>
         <v>2. 休假由生病天數:.天(截至日期2025/03/10)</v>
       </c>
       <c r="B27" s="51"/>
@@ -6583,13 +6551,13 @@
     </row>
     <row r="28" spans="1:36">
       <c r="A28" s="34" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="B28" s="34"/>
       <c r="C28" s="34"/>
       <c r="D28" s="34"/>
       <c r="E28" s="34" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F28" s="34"/>
       <c r="G28" s="34"/>
@@ -6609,7 +6577,7 @@
       <c r="S28" s="34"/>
       <c r="T28" s="34"/>
       <c r="U28" s="34" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="V28" s="34"/>
       <c r="W28" s="34"/>
@@ -6631,75 +6599,75 @@
     </row>
     <row r="29" spans="1:36" ht="81.75" customHeight="1">
       <c r="A29" s="39" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="B29" s="39"/>
       <c r="C29" s="39" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="D29" s="39"/>
       <c r="E29" s="39" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="F29" s="39"/>
       <c r="G29" s="39" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="H29" s="39"/>
       <c r="I29" s="39" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="J29" s="39"/>
       <c r="K29" s="39" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="L29" s="39"/>
       <c r="M29" s="39" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="N29" s="39"/>
       <c r="O29" s="39" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="P29" s="39"/>
       <c r="Q29" s="39" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="R29" s="39"/>
       <c r="S29" s="39" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="T29" s="39"/>
       <c r="U29" s="39" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="V29" s="39"/>
       <c r="W29" s="39" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="X29" s="39"/>
       <c r="Y29" s="39" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="Z29" s="39"/>
       <c r="AA29" s="39" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="AB29" s="39"/>
       <c r="AC29" s="39" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="AD29" s="39"/>
       <c r="AE29" s="39" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="AF29" s="39"/>
       <c r="AG29" s="39" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="AH29" s="39"/>
       <c r="AI29" s="39" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="AJ29" s="39"/>
     </row>
@@ -6707,77 +6675,77 @@
       <c r="A30" s="39"/>
       <c r="B30" s="39"/>
       <c r="C30" s="44" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="D30" s="39"/>
       <c r="E30" s="44" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="F30" s="39"/>
       <c r="G30" s="44" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="H30" s="39"/>
       <c r="I30" s="44" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="J30" s="39"/>
       <c r="K30" s="44" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="L30" s="39"/>
       <c r="M30" s="44" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="N30" s="39"/>
       <c r="O30" s="44" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="P30" s="39"/>
       <c r="Q30" s="44" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="R30" s="39"/>
       <c r="S30" s="44" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="T30" s="39"/>
       <c r="U30" s="44" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="V30" s="39"/>
       <c r="W30" s="44" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="X30" s="39"/>
       <c r="Y30" s="44" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="Z30" s="39"/>
       <c r="AA30" s="44" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="AB30" s="39"/>
       <c r="AC30" s="44" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="AD30" s="39"/>
       <c r="AE30" s="44" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="AF30" s="39"/>
       <c r="AG30" s="44" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="AH30" s="39"/>
       <c r="AI30" s="44" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="AJ30" s="39"/>
     </row>
     <row r="31" spans="1:36">
       <c r="A31" s="39" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B31" s="39"/>
       <c r="C31" s="46">
@@ -7043,7 +7011,7 @@
     </row>
     <row r="34" spans="1:36">
       <c r="A34" s="39" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B34" s="39"/>
       <c r="C34" s="46">
@@ -7309,7 +7277,7 @@
     </row>
     <row r="37" spans="1:36">
       <c r="A37" s="39" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B37" s="39"/>
       <c r="C37" s="46">
@@ -7575,7 +7543,7 @@
     </row>
     <row r="40" spans="1:36">
       <c r="A40" s="39" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B40" s="39"/>
       <c r="C40" s="46">
@@ -7929,7 +7897,7 @@
     </row>
     <row r="45" spans="1:36">
       <c r="A45" s="45" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B45" s="45"/>
       <c r="C45" s="45"/>
@@ -7969,7 +7937,7 @@
     </row>
     <row r="46" spans="1:36" s="26" customFormat="1" ht="81" customHeight="1">
       <c r="A46" s="42" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B46" s="43"/>
       <c r="C46" s="43"/>
@@ -8126,10 +8094,6 @@
     <mergeCell ref="S11:T11"/>
     <mergeCell ref="U11:V11"/>
     <mergeCell ref="W11:X11"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
     <mergeCell ref="K13:L13"/>
     <mergeCell ref="W12:X12"/>
     <mergeCell ref="Y12:Z12"/>
@@ -8162,6 +8126,10 @@
     <mergeCell ref="Q14:R14"/>
     <mergeCell ref="S14:T14"/>
     <mergeCell ref="U14:V14"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
     <mergeCell ref="M15:N15"/>
     <mergeCell ref="O15:P15"/>
     <mergeCell ref="Q15:R15"/>
@@ -8566,7 +8534,7 @@
   <dimension ref="A1:AD14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AF5" sqref="AF5"/>
+      <selection activeCell="AE3" sqref="AE3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -10230,8 +10198,9 @@
       <c r="M3" s="80"/>
       <c r="N3" s="80"/>
       <c r="O3" s="80"/>
-      <c r="P3" s="81" t="s">
-        <v>140</v>
+      <c r="P3" s="81" t="str">
+        <f ca="1">CONCATENATE("CẬP NHẬT: ",TEXT(TODAY(),"dd/MM/yyyy"))</f>
+        <v>CẬP NHẬT: 10/03/2025</v>
       </c>
       <c r="Q3" s="81"/>
       <c r="R3" s="81"/>
@@ -10261,12 +10230,24 @@
       <c r="J4" s="39"/>
       <c r="K4" s="39"/>
       <c r="L4" s="39"/>
-      <c r="M4" s="22"/>
+      <c r="M4" s="22">
+        <v>0</v>
+      </c>
       <c r="N4" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="O4" s="86" t="s">
-        <v>141</v>
+      <c r="O4" s="86" t="str">
+        <f>CONCATENATE("Nguyên nhân chưa khám sức khỏe:",CHAR(10),"(1) Nghỉ việc ",AC4," (H)
+(2) Không tại chức: ",M10," (G)
+(3) Thời gian chưa điều chuyển: ",AC5," (I)
+(4) Về đài: ",AC6," (J)
+(5) Khác: ",AC7," (K)")</f>
+        <v>Nguyên nhân chưa khám sức khỏe:
+(1) Nghỉ việc 0 (H)
+(2) Không tại chức: 0 (G)
+(3) Thời gian chưa điều chuyển: 0 (I)
+(4) Về đài: 0 (J)
+(5) Khác: 0 (K)</v>
       </c>
       <c r="P4" s="87"/>
       <c r="Q4" s="87"/>
@@ -10274,7 +10255,7 @@
       <c r="S4" s="87"/>
       <c r="T4" s="88"/>
       <c r="U4" s="86" t="s">
-        <v>144</v>
+        <v>210</v>
       </c>
       <c r="V4" s="87"/>
       <c r="W4" s="87"/>
@@ -10282,9 +10263,11 @@
       <c r="Y4" s="87"/>
       <c r="Z4" s="88"/>
       <c r="AB4" s="27" t="s">
-        <v>215</v>
-      </c>
-      <c r="AC4" s="27"/>
+        <v>207</v>
+      </c>
+      <c r="AC4" s="27">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:29" s="24" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A5" s="22">
@@ -10303,7 +10286,9 @@
       <c r="J5" s="82"/>
       <c r="K5" s="82"/>
       <c r="L5" s="82"/>
-      <c r="M5" s="22"/>
+      <c r="M5" s="22">
+        <v>0</v>
+      </c>
       <c r="N5" s="22" t="s">
         <v>128</v>
       </c>
@@ -10322,7 +10307,9 @@
       <c r="AB5" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="AC5" s="27"/>
+      <c r="AC5" s="27">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:29" s="24" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A6" s="22">
@@ -10341,7 +10328,9 @@
       <c r="J6" s="82"/>
       <c r="K6" s="82"/>
       <c r="L6" s="82"/>
-      <c r="M6" s="22"/>
+      <c r="M6" s="22">
+        <v>0</v>
+      </c>
       <c r="N6" s="22" t="s">
         <v>130</v>
       </c>
@@ -10358,9 +10347,11 @@
       <c r="Y6" s="90"/>
       <c r="Z6" s="91"/>
       <c r="AB6" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="AC6" s="27"/>
+        <v>208</v>
+      </c>
+      <c r="AC6" s="27">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:29" s="24" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A7" s="22">
@@ -10379,7 +10370,9 @@
       <c r="J7" s="82"/>
       <c r="K7" s="82"/>
       <c r="L7" s="82"/>
-      <c r="M7" s="22"/>
+      <c r="M7" s="22">
+        <v>0</v>
+      </c>
       <c r="N7" s="22" t="s">
         <v>132</v>
       </c>
@@ -10396,16 +10389,18 @@
       <c r="Y7" s="90"/>
       <c r="Z7" s="91"/>
       <c r="AB7" s="27" t="s">
-        <v>217</v>
-      </c>
-      <c r="AC7" s="27"/>
+        <v>209</v>
+      </c>
+      <c r="AC7" s="27">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:29" s="24" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A8" s="22">
         <v>5</v>
       </c>
       <c r="B8" s="82" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C8" s="82"/>
       <c r="D8" s="82"/>
@@ -10442,7 +10437,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="82" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C9" s="82"/>
       <c r="D9" s="82"/>
@@ -10454,12 +10449,19 @@
       <c r="J9" s="82"/>
       <c r="K9" s="82"/>
       <c r="L9" s="82"/>
-      <c r="M9" s="22"/>
+      <c r="M9" s="22">
+        <v>0</v>
+      </c>
       <c r="N9" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="O9" s="86" t="s">
-        <v>142</v>
+      <c r="O9" s="86" t="str">
+        <f>CONCATENATE("Phương án xử lí
+(1) Không thể khám bù: ",AC4+M10," (H+G)
+(2) Có thể khám bù: ",AC5+AC6+AC7," (I+J+K)")</f>
+        <v>Phương án xử lí
+(1) Không thể khám bù: 0 (H+G)
+(2) Có thể khám bù: 0 (I+J+K)</v>
       </c>
       <c r="P9" s="87"/>
       <c r="Q9" s="87"/>
@@ -10467,7 +10469,7 @@
       <c r="S9" s="87"/>
       <c r="T9" s="88"/>
       <c r="U9" s="86" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="V9" s="87"/>
       <c r="W9" s="87"/>
@@ -10480,7 +10482,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="82" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C10" s="82"/>
       <c r="D10" s="82"/>
@@ -10492,7 +10494,9 @@
       <c r="J10" s="82"/>
       <c r="K10" s="82"/>
       <c r="L10" s="82"/>
-      <c r="M10" s="22"/>
+      <c r="M10" s="22">
+        <v>0</v>
+      </c>
       <c r="N10" s="22" t="s">
         <v>135</v>
       </c>
@@ -10514,7 +10518,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="82" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C11" s="82"/>
       <c r="D11" s="82"/>
@@ -10526,7 +10530,9 @@
       <c r="J11" s="82"/>
       <c r="K11" s="82"/>
       <c r="L11" s="82"/>
-      <c r="M11" s="22"/>
+      <c r="M11" s="22">
+        <v>0</v>
+      </c>
       <c r="N11" s="22" t="s">
         <v>136</v>
       </c>
@@ -10548,7 +10554,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="82" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C12" s="82"/>
       <c r="D12" s="82"/>
@@ -10560,7 +10566,9 @@
       <c r="J12" s="82"/>
       <c r="K12" s="82"/>
       <c r="L12" s="82"/>
-      <c r="M12" s="22"/>
+      <c r="M12" s="22">
+        <v>0</v>
+      </c>
       <c r="N12" s="22"/>
       <c r="O12" s="92"/>
       <c r="P12" s="93"/>
@@ -10577,7 +10585,7 @@
     </row>
     <row r="13" spans="1:29" ht="101.25" customHeight="1">
       <c r="A13" s="84" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B13" s="85"/>
       <c r="C13" s="85"/>
@@ -10639,7 +10647,7 @@
     </row>
     <row r="15" spans="1:29" ht="34.5" customHeight="1">
       <c r="A15" s="79" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B15" s="79"/>
       <c r="C15" s="79"/>
@@ -10670,7 +10678,7 @@
     <row r="16" spans="1:29" ht="20.100000000000001" customHeight="1"/>
     <row r="17" spans="1:26" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="80" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B17" s="80"/>
       <c r="C17" s="80"/>
@@ -10686,8 +10694,9 @@
       <c r="M17" s="80"/>
       <c r="N17" s="80"/>
       <c r="O17" s="80"/>
-      <c r="P17" s="81" t="s">
-        <v>160</v>
+      <c r="P17" s="81" t="str">
+        <f ca="1">CONCATENATE("更新日期:",TEXT(TODAY(),"yyyy/MM/dd"))</f>
+        <v>更新日期:2025/03/10</v>
       </c>
       <c r="Q17" s="81"/>
       <c r="R17" s="81"/>
@@ -10705,37 +10714,37 @@
         <v>1</v>
       </c>
       <c r="B18" s="82" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C18" s="82" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D18" s="82" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E18" s="82" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F18" s="82" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G18" s="82" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H18" s="82" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I18" s="82" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="J18" s="82" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="K18" s="82" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="L18" s="82" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="M18" s="22">
         <f>M4</f>
@@ -10744,8 +10753,19 @@
       <c r="N18" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="O18" s="86" t="s">
-        <v>161</v>
+      <c r="O18" s="86" t="str">
+        <f>CONCATENATE("應健檢而未健檢原因分析：
+（1）離職： ",AC4,"（H）
+（2）未在職：",M10,"（G)
+（3）未調換時間：",AC5,"（I)
+（4）返台：",AC6,"（J)
+（5）其他：",AC7,"（K)")</f>
+        <v>應健檢而未健檢原因分析：
+（1）離職： 0（H）
+（2）未在職：0（G)
+（3）未調換時間：0（I)
+（4）返台：0（J)
+（5）其他：0（K)</v>
       </c>
       <c r="P18" s="87"/>
       <c r="Q18" s="87"/>
@@ -10753,7 +10773,7 @@
       <c r="S18" s="87"/>
       <c r="T18" s="88"/>
       <c r="U18" s="86" t="s">
-        <v>162</v>
+        <v>211</v>
       </c>
       <c r="V18" s="87"/>
       <c r="W18" s="87"/>
@@ -10766,37 +10786,37 @@
         <v>2</v>
       </c>
       <c r="B19" s="82" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C19" s="82" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D19" s="82" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E19" s="82" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F19" s="82" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="G19" s="82" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H19" s="82" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="I19" s="82" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="J19" s="82" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K19" s="82" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="L19" s="82" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="M19" s="27">
         <f t="shared" ref="M19:M26" si="0">M5</f>
@@ -10823,37 +10843,37 @@
         <v>3</v>
       </c>
       <c r="B20" s="82" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C20" s="82" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D20" s="82" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E20" s="82" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F20" s="82" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="G20" s="82" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="H20" s="82" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I20" s="82" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="J20" s="82" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K20" s="82" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="L20" s="82" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="M20" s="27">
         <f t="shared" si="0"/>
@@ -10880,37 +10900,37 @@
         <v>4</v>
       </c>
       <c r="B21" s="82" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C21" s="82" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D21" s="82" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E21" s="82" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F21" s="82" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="G21" s="82" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H21" s="82" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="I21" s="82" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J21" s="82" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="K21" s="82" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="L21" s="82" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="M21" s="27">
         <f t="shared" si="0"/>
@@ -10937,37 +10957,37 @@
         <v>5</v>
       </c>
       <c r="B22" s="82" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C22" s="82" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D22" s="82" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E22" s="82" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F22" s="82" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G22" s="82" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="H22" s="82" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="I22" s="82" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="J22" s="82" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="K22" s="82" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="L22" s="82" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="M22" s="27">
         <f t="shared" si="0"/>
@@ -10994,37 +11014,37 @@
         <v>6</v>
       </c>
       <c r="B23" s="82" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C23" s="82" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="D23" s="82" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="E23" s="82" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="F23" s="82" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="G23" s="82" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="H23" s="82" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="I23" s="82" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="J23" s="82" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="K23" s="82" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="L23" s="82" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="M23" s="27">
         <f t="shared" si="0"/>
@@ -11033,8 +11053,13 @@
       <c r="N23" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="O23" s="86" t="s">
-        <v>163</v>
+      <c r="O23" s="86" t="str">
+        <f>CONCATENATE("應健檢而未檢查處理
+（1）不可補檢：",AC4+M10," (H+G)
+（2）可補檢：",AC5+AC6+AC7," (I+J+K)")</f>
+        <v>應健檢而未檢查處理
+（1）不可補檢：0 (H+G)
+（2）可補檢：0 (I+J+K)</v>
       </c>
       <c r="P23" s="87"/>
       <c r="Q23" s="87"/>
@@ -11042,7 +11067,7 @@
       <c r="S23" s="87"/>
       <c r="T23" s="88"/>
       <c r="U23" s="86" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="V23" s="87"/>
       <c r="W23" s="87"/>
@@ -11055,37 +11080,37 @@
         <v>7</v>
       </c>
       <c r="B24" s="82" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C24" s="82" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D24" s="82" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E24" s="82" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F24" s="82" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G24" s="82" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H24" s="82" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="I24" s="82" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="J24" s="82" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="K24" s="82" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="L24" s="82" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="M24" s="27">
         <f t="shared" si="0"/>
@@ -11112,37 +11137,37 @@
         <v>8</v>
       </c>
       <c r="B25" s="82" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C25" s="82" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D25" s="82" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E25" s="82" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F25" s="82" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G25" s="82" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H25" s="82" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="I25" s="82" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="J25" s="82" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="K25" s="82" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="L25" s="82" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="M25" s="27">
         <f t="shared" si="0"/>
@@ -11169,37 +11194,37 @@
         <v>9</v>
       </c>
       <c r="B26" s="82" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C26" s="82" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D26" s="82" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E26" s="82" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F26" s="82" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G26" s="82" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="H26" s="82" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="I26" s="82" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="J26" s="82" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="K26" s="82" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="L26" s="82" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="M26" s="27">
         <f t="shared" si="0"/>
@@ -11221,7 +11246,7 @@
     </row>
     <row r="27" spans="1:26" ht="101.25" customHeight="1">
       <c r="A27" s="84" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B27" s="85"/>
       <c r="C27" s="85"/>
@@ -11251,7 +11276,7 @@
     </row>
     <row r="28" spans="1:26" ht="20.100000000000001" customHeight="1">
       <c r="A28" s="83" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B28" s="83"/>
       <c r="C28" s="83"/>
@@ -11266,7 +11291,7 @@
       <c r="L28" s="83"/>
       <c r="M28" s="83"/>
       <c r="N28" s="83" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="O28" s="83"/>
       <c r="P28" s="83"/>

</xml_diff>